<commit_message>
Cambios de la tercara infografía
Grafícos y Tableau
</commit_message>
<xml_diff>
--- a/data/Datos 3era Infografía.xlsx
+++ b/data/Datos 3era Infografía.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Actividades de innovacion" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Factores Alto No I+D" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Factores de no Innovar'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Factores de no Innovar'!$A$1:$F$23</definedName>
   </definedNames>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="252">
   <si>
     <t>Actividad</t>
   </si>
@@ -682,13 +682,121 @@
   </si>
   <si>
     <t>60.4</t>
+  </si>
+  <si>
+    <t>{name:'Pequeñas',  data:[</t>
+  </si>
+  <si>
+    <t>0.86,</t>
+  </si>
+  <si>
+    <t>0.73,</t>
+  </si>
+  <si>
+    <t>1.3,</t>
+  </si>
+  <si>
+    <t>1.4]},</t>
+  </si>
+  <si>
+    <t>{name:'Medianas',  data:[</t>
+  </si>
+  <si>
+    <t>0.43,</t>
+  </si>
+  <si>
+    <t>0.44,</t>
+  </si>
+  <si>
+    <t>1.1,</t>
+  </si>
+  <si>
+    <t>1]},</t>
+  </si>
+  <si>
+    <t>{name:'Grandes',  data:[</t>
+  </si>
+  <si>
+    <t>0.36,</t>
+  </si>
+  <si>
+    <t>0.3,</t>
+  </si>
+  <si>
+    <t>0.72,</t>
+  </si>
+  <si>
+    <t>1.2]},</t>
+  </si>
+  <si>
+    <t>55.5</t>
+  </si>
+  <si>
+    <t>49.2</t>
+  </si>
+  <si>
+    <t>48.8</t>
+  </si>
+  <si>
+    <t>42.1</t>
+  </si>
+  <si>
+    <t>45.6</t>
+  </si>
+  <si>
+    <t>43.8</t>
+  </si>
+  <si>
+    <t>44.0</t>
+  </si>
+  <si>
+    <t>37.4</t>
+  </si>
+  <si>
+    <t>32.4</t>
+  </si>
+  <si>
+    <t>38.0</t>
+  </si>
+  <si>
+    <t>21.5</t>
+  </si>
+  <si>
+    <t>17.4</t>
+  </si>
+  <si>
+    <t>13.4</t>
+  </si>
+  <si>
+    <t>10.4</t>
+  </si>
+  <si>
+    <t>6.4</t>
+  </si>
+  <si>
+    <t>38.5</t>
+  </si>
+  <si>
+    <t>33.3</t>
+  </si>
+  <si>
+    <t>43.3</t>
+  </si>
+  <si>
+    <t>33.4</t>
+  </si>
+  <si>
+    <t>26.7</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -708,6 +816,14 @@
       <color rgb="FF000000"/>
       <name val="Cambria"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -742,7 +858,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -752,6 +868,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1802,13 +1922,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2102,8 +2222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2854,39 +2974,39 @@
         <v>{name:'A cualquier tipo de innovación',  data:[</v>
       </c>
       <c r="B33" t="str">
-        <f>B26&amp;","</f>
+        <f t="shared" ref="B33:J33" si="5">B26&amp;","</f>
         <v>17.3,</v>
       </c>
       <c r="C33" t="str">
-        <f>C26&amp;","</f>
+        <f t="shared" si="5"/>
         <v>22.7,</v>
       </c>
       <c r="D33" t="str">
-        <f>D26&amp;","</f>
+        <f t="shared" si="5"/>
         <v>27.7,</v>
       </c>
       <c r="E33" t="str">
-        <f>E26&amp;","</f>
+        <f t="shared" si="5"/>
         <v>29.1,</v>
       </c>
       <c r="F33" t="str">
-        <f>F26&amp;","</f>
+        <f t="shared" si="5"/>
         <v>38.3,</v>
       </c>
       <c r="G33" t="str">
-        <f>G26&amp;","</f>
+        <f t="shared" si="5"/>
         <v>44.1,</v>
       </c>
       <c r="H33" t="str">
-        <f>H26&amp;","</f>
+        <f t="shared" si="5"/>
         <v>48.9,</v>
       </c>
       <c r="I33" t="str">
-        <f>I26&amp;","</f>
+        <f t="shared" si="5"/>
         <v>57.4,</v>
       </c>
       <c r="J33" t="str">
-        <f>J26&amp;","</f>
+        <f t="shared" si="5"/>
         <v>66.6,</v>
       </c>
       <c r="K33" t="str">
@@ -2900,39 +3020,39 @@
         <v>{name:'Producto',  data:[</v>
       </c>
       <c r="B34" t="str">
-        <f>B27&amp;","</f>
+        <f t="shared" ref="B34:J34" si="6">B27&amp;","</f>
         <v>58.1,</v>
       </c>
       <c r="C34" t="str">
-        <f>C27&amp;","</f>
+        <f t="shared" si="6"/>
         <v>13.3,</v>
       </c>
       <c r="D34" t="str">
-        <f>D27&amp;","</f>
+        <f t="shared" si="6"/>
         <v>29.5,</v>
       </c>
       <c r="E34" t="str">
-        <f>E27&amp;","</f>
+        <f t="shared" si="6"/>
         <v>13.1,</v>
       </c>
       <c r="F34" t="str">
-        <f>F27&amp;","</f>
+        <f t="shared" si="6"/>
         <v>12.8,</v>
       </c>
       <c r="G34" t="str">
-        <f>G27&amp;","</f>
+        <f t="shared" si="6"/>
         <v>17.3,</v>
       </c>
       <c r="H34" t="str">
-        <f>H27&amp;","</f>
+        <f t="shared" si="6"/>
         <v>16.7,</v>
       </c>
       <c r="I34" t="str">
-        <f>I27&amp;","</f>
+        <f t="shared" si="6"/>
         <v>22.7,</v>
       </c>
       <c r="J34" t="str">
-        <f>J27&amp;","</f>
+        <f t="shared" si="6"/>
         <v>32.9,</v>
       </c>
       <c r="K34" t="str">
@@ -2946,39 +3066,39 @@
         <v>{name:'Proceso',  data:[</v>
       </c>
       <c r="B35" t="str">
-        <f>B28&amp;","</f>
+        <f t="shared" ref="B35:J35" si="7">B28&amp;","</f>
         <v>43.9,</v>
       </c>
       <c r="C35" t="str">
-        <f>C28&amp;","</f>
+        <f t="shared" si="7"/>
         <v>7,</v>
       </c>
       <c r="D35" t="str">
-        <f>D28&amp;","</f>
+        <f t="shared" si="7"/>
         <v>44.6,</v>
       </c>
       <c r="E35" t="str">
-        <f>E28&amp;","</f>
+        <f t="shared" si="7"/>
         <v>24.3,</v>
       </c>
       <c r="F35" t="str">
-        <f>F28&amp;","</f>
+        <f t="shared" si="7"/>
         <v>24.3,</v>
       </c>
       <c r="G35" t="str">
-        <f>G28&amp;","</f>
+        <f t="shared" si="7"/>
         <v>18.2,</v>
       </c>
       <c r="H35" t="str">
-        <f>H28&amp;","</f>
+        <f t="shared" si="7"/>
         <v>21.6,</v>
       </c>
       <c r="I35" t="str">
-        <f>I28&amp;","</f>
+        <f t="shared" si="7"/>
         <v>27.3,</v>
       </c>
       <c r="J35" t="str">
-        <f>J28&amp;","</f>
+        <f t="shared" si="7"/>
         <v>46.6,</v>
       </c>
       <c r="K35" t="str">
@@ -2992,39 +3112,39 @@
         <v>{name:'Organización',  data:[</v>
       </c>
       <c r="B36" t="str">
-        <f>B29&amp;","</f>
+        <f t="shared" ref="B36:J36" si="8">B29&amp;","</f>
         <v>20.3,</v>
       </c>
       <c r="C36" t="str">
-        <f>C29&amp;","</f>
+        <f t="shared" si="8"/>
         <v>2.3,</v>
       </c>
       <c r="D36" t="str">
-        <f>D29&amp;","</f>
+        <f t="shared" si="8"/>
         <v>7.9,</v>
       </c>
       <c r="E36" t="str">
-        <f>E29&amp;","</f>
+        <f t="shared" si="8"/>
         <v>28.8,</v>
       </c>
       <c r="F36" t="str">
-        <f>F29&amp;","</f>
+        <f t="shared" si="8"/>
         <v>26.8,</v>
       </c>
       <c r="G36" t="str">
-        <f>G29&amp;","</f>
+        <f t="shared" si="8"/>
         <v>9.9,</v>
       </c>
       <c r="H36" t="str">
-        <f>H29&amp;","</f>
+        <f t="shared" si="8"/>
         <v>6.1,</v>
       </c>
       <c r="I36" t="str">
-        <f>I29&amp;","</f>
+        <f t="shared" si="8"/>
         <v>18.2,</v>
       </c>
       <c r="J36" t="str">
-        <f>J29&amp;","</f>
+        <f t="shared" si="8"/>
         <v>35.4,</v>
       </c>
       <c r="K36" t="str">
@@ -3038,39 +3158,39 @@
         <v>{name:'Comercialización',  data:[</v>
       </c>
       <c r="B37" t="str">
-        <f>B30&amp;","</f>
+        <f t="shared" ref="B37:J37" si="9">B30&amp;","</f>
         <v>25.9,</v>
       </c>
       <c r="C37" t="str">
-        <f>C30&amp;","</f>
+        <f t="shared" si="9"/>
         <v>6.3,</v>
       </c>
       <c r="D37" t="str">
-        <f>D30&amp;","</f>
+        <f t="shared" si="9"/>
         <v>9.2,</v>
       </c>
       <c r="E37" t="str">
-        <f>E30&amp;","</f>
+        <f t="shared" si="9"/>
         <v>17.6,</v>
       </c>
       <c r="F37" t="str">
-        <f>F30&amp;","</f>
+        <f t="shared" si="9"/>
         <v>16.7,</v>
       </c>
       <c r="G37" t="str">
-        <f>G30&amp;","</f>
+        <f t="shared" si="9"/>
         <v>6.8,</v>
       </c>
       <c r="H37" t="str">
-        <f>H30&amp;","</f>
+        <f t="shared" si="9"/>
         <v>4.5,</v>
       </c>
       <c r="I37" t="str">
-        <f>I30&amp;","</f>
+        <f t="shared" si="9"/>
         <v>11.5,</v>
       </c>
       <c r="J37" t="str">
-        <f>J30&amp;","</f>
+        <f t="shared" si="9"/>
         <v>22.7,</v>
       </c>
       <c r="K37" t="str">
@@ -3087,8 +3207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:Q27"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3778,7 +3898,7 @@
         <v>65.6,</v>
       </c>
       <c r="C28" t="str">
-        <f t="shared" ref="C28:Q28" si="1">C22&amp;","</f>
+        <f t="shared" ref="C28:P28" si="1">C22&amp;","</f>
         <v>49.8,</v>
       </c>
       <c r="D28" t="str">
@@ -3844,7 +3964,7 @@
         <v>{name:'Media',  data:[</v>
       </c>
       <c r="B29" t="str">
-        <f t="shared" ref="B29:Q31" si="3">B23&amp;","</f>
+        <f t="shared" ref="B29:P31" si="3">B23&amp;","</f>
         <v>20.4,</v>
       </c>
       <c r="C29" t="str">
@@ -4055,10 +4175,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4134,6 +4254,57 @@
         <v>1.2</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>216</v>
+      </c>
+      <c r="B7" t="s">
+        <v>217</v>
+      </c>
+      <c r="C7" t="s">
+        <v>218</v>
+      </c>
+      <c r="D7" t="s">
+        <v>219</v>
+      </c>
+      <c r="E7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B8" t="s">
+        <v>222</v>
+      </c>
+      <c r="C8" t="s">
+        <v>223</v>
+      </c>
+      <c r="D8" t="s">
+        <v>224</v>
+      </c>
+      <c r="E8" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>226</v>
+      </c>
+      <c r="B9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D9" t="s">
+        <v>229</v>
+      </c>
+      <c r="E9" t="s">
+        <v>230</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4142,16 +4313,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="48" x14ac:dyDescent="0.25">
@@ -4175,447 +4350,453 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="4">
         <v>26.6</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="4">
         <v>63.4</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="4">
         <v>41</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="4">
         <v>51.3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="4">
         <v>20</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="4">
         <v>70</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="4">
         <v>38.5</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="4">
         <v>53.8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>26.7</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>63.3</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <v>33.299999999999997</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="4">
         <v>58.9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="4">
         <v>23.3</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="4">
         <v>66.7</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="4">
         <v>33.299999999999997</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="4">
         <v>58.9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="4">
         <v>16.7</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <v>73.400000000000006</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="4">
         <v>33.299999999999997</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="4">
         <v>58.9</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="4">
         <v>33.4</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="4">
         <v>56.7</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="4">
         <v>30.7</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="4">
         <v>61.5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="4">
         <v>23.3</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="4">
         <v>66.7</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="4">
         <v>30.7</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="4">
         <v>61.6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="4">
         <v>23.3</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="4">
         <v>66.599999999999994</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="4">
         <v>30.7</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="4">
         <v>61.6</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="4">
         <v>26.6</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="4">
         <v>63.3</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="4">
         <v>28.2</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="4">
         <v>64.099999999999994</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="4">
         <v>26.6</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="4">
         <v>63.3</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="4">
         <v>25.6</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="4">
         <v>66.599999999999994</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4">
         <v>30</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="4">
         <v>60</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="4">
         <v>23.1</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="4">
         <v>69.2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="4">
         <v>26.7</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="4">
         <v>63.4</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="4">
         <v>23.1</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="4">
         <v>69.2</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="4">
         <v>20</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="4">
         <v>70</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="4">
         <v>23.1</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="4">
         <v>69.3</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="4">
         <v>43.3</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="4">
         <v>46.7</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="4">
         <v>20.5</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="4">
         <v>71.8</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4">
         <v>13.4</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="4">
         <v>74.3</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="4">
         <v>18</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="4">
         <v>74.3</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="4">
         <v>23.3</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="4">
         <v>66.7</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="4">
         <v>17.899999999999999</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="4">
         <v>74.400000000000006</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <v>26.7</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="4">
         <v>63.3</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="4">
         <v>15.4</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="4">
         <v>76.900000000000006</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="4">
         <v>20</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="4">
         <v>70</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="4">
         <v>15.4</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="4">
         <v>76.900000000000006</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="4">
         <v>3.3</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="4">
         <v>86.6</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="4">
         <v>15.4</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="4">
         <v>76.900000000000006</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="4">
         <v>16.7</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="4">
         <v>73.3</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="4">
         <v>5.2</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="4">
         <v>87.2</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="4">
         <v>10</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="4">
         <v>80</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="4">
         <v>5.0999999999999996</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="4">
         <v>87.2</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="4">
         <v>30</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="4">
         <v>60</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="4">
         <v>2.6</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="4">
         <v>89.8</v>
       </c>
     </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="str">
+        <f>"{name:'"&amp;B2&amp;"',  data:["</f>
+        <v>{name:'Carencia de infraestructura física',  data:[</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F1">
+  <autoFilter ref="A1:F23">
     <sortState ref="A2:F23">
       <sortCondition descending="1" ref="E1"/>
     </sortState>
@@ -4633,15 +4814,16 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B13" sqref="B13:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4650,7 +4832,7 @@
     <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -4658,44 +4840,135 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B3">
-        <v>38.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B3" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B4">
-        <v>33.299999999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B4" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B5">
-        <v>33.299999999999997</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B5" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B6">
-        <v>33.299999999999997</v>
+      <c r="B6" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="5">
+        <v>41</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="str">
+        <f>"'"&amp;B10&amp;"',"</f>
+        <v>'Carencia de infraestructura física',</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" ref="C13:H13" si="0">"'"&amp;C10&amp;"',"</f>
+        <v>'Escaso desarrollo de instituciones relacionadas con ciencia y tecnología',</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>'Reducido tamaño del mercado',</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>'Políticas públicas inadecuadas para la promoción de C&amp;T',</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>'Períodos de retorno inconvenientes',</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f>"{name:'"&amp;A11&amp;"',  data:["</f>
+        <v>{name:'Factor',  data:[</v>
+      </c>
+      <c r="B14" t="str">
+        <f>B11&amp;","</f>
+        <v>41,</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" ref="C14:F14" si="1">C11&amp;","</f>
+        <v>38.5,</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>33.3,</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>33.3,</v>
+      </c>
+      <c r="F14" t="str">
+        <f>F11&amp;"]}"</f>
+        <v>33.3]}</v>
       </c>
     </row>
   </sheetData>
@@ -4705,19 +4978,19 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" customWidth="1"/>
+    <col min="1" max="1" width="51.7109375" customWidth="1"/>
     <col min="2" max="2" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -4725,44 +4998,132 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
-      <c r="B2">
-        <v>43.3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
       </c>
-      <c r="B3">
-        <v>33.4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
-      <c r="B6">
-        <v>26.7</v>
+      <c r="B6" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="D11" s="5">
+        <v>30</v>
+      </c>
+      <c r="E11" s="5">
+        <v>30</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="str">
+        <f>"'"&amp;B10&amp;"',"</f>
+        <v>'Falta de recursos financieros propios',</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" ref="C13:F13" si="0">"'"&amp;C10&amp;"',"</f>
+        <v>'Facilidad de imitación por terceros',</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>'Escasez de personal capacitado',</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>'No consideraron necesario hacer ninguna innovación',</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>'Reducido tamaño del mercado',</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f>"{name:'"&amp;A11&amp;"',  data:["</f>
+        <v>{name:'Porcentaje',  data:[</v>
+      </c>
+      <c r="B14" t="str">
+        <f>B11&amp;","</f>
+        <v>43.3,</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" ref="C14:F14" si="1">C11&amp;","</f>
+        <v>33.4,</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>30,</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>30,</v>
+      </c>
+      <c r="F14" t="str">
+        <f>F11&amp;"]}"</f>
+        <v>26.7]}</v>
       </c>
     </row>
   </sheetData>
@@ -4775,14 +5136,15 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E12"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="1" max="1" width="47" customWidth="1"/>
     <col min="2" max="2" width="23.140625" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -4996,16 +5358,16 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="75.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -5140,6 +5502,266 @@
         <v>123</v>
       </c>
     </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" t="s">
+        <v>86</v>
+      </c>
+      <c r="F18" t="s">
+        <v>89</v>
+      </c>
+      <c r="G18" t="s">
+        <v>92</v>
+      </c>
+      <c r="H18" t="s">
+        <v>95</v>
+      </c>
+      <c r="I18" t="s">
+        <v>98</v>
+      </c>
+      <c r="J18" t="s">
+        <v>101</v>
+      </c>
+      <c r="K18" t="s">
+        <v>104</v>
+      </c>
+      <c r="L18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" t="s">
+        <v>231</v>
+      </c>
+      <c r="D19" t="s">
+        <v>233</v>
+      </c>
+      <c r="E19" t="s">
+        <v>235</v>
+      </c>
+      <c r="F19" t="s">
+        <v>236</v>
+      </c>
+      <c r="G19" t="s">
+        <v>238</v>
+      </c>
+      <c r="H19" t="s">
+        <v>239</v>
+      </c>
+      <c r="I19" t="s">
+        <v>241</v>
+      </c>
+      <c r="J19" t="s">
+        <v>242</v>
+      </c>
+      <c r="K19" t="s">
+        <v>243</v>
+      </c>
+      <c r="L19" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" t="s">
+        <v>232</v>
+      </c>
+      <c r="D20" t="s">
+        <v>234</v>
+      </c>
+      <c r="E20" t="s">
+        <v>192</v>
+      </c>
+      <c r="F20" t="s">
+        <v>237</v>
+      </c>
+      <c r="G20" t="s">
+        <v>192</v>
+      </c>
+      <c r="H20" t="s">
+        <v>240</v>
+      </c>
+      <c r="I20" t="s">
+        <v>192</v>
+      </c>
+      <c r="J20" t="s">
+        <v>177</v>
+      </c>
+      <c r="K20" t="s">
+        <v>151</v>
+      </c>
+      <c r="L20" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B26" t="str">
+        <f>"'"&amp;B18&amp;"',"</f>
+        <v>'I+D es demasiado caro para la empresa',</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" ref="C26:L26" si="0">"'"&amp;C18&amp;"',"</f>
+        <v>'Falta de apoyo del Sector Público',</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="0"/>
+        <v>'Falta de acceso a crédito',</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="0"/>
+        <v>'Las fuentes externas de información son suficientes para la innovación',</v>
+      </c>
+      <c r="F26" t="str">
+        <f t="shared" si="0"/>
+        <v>'Mercados pequeños que no permiten la recuperación de las inversiones en I+D',</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v>'Las inversiones en I+D son muy riesgosas',</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="0"/>
+        <v>'Dificultades para apropiarse de los resultados de la I+D',</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="0"/>
+        <v>'I+D no es necesario para las actividades de innovación de la empresa',</v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" si="0"/>
+        <v>'La empresa no innova',</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="0"/>
+        <v>'Las universidades substituyen la I+D de la empresa',</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="0"/>
+        <v>'Los centros e institutos de investigación públicos substituyen la I+D de la empresa',</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f>"{name:'"&amp;A19&amp;"',  data:["</f>
+        <v>{name:'Empresas que Invirtieron en I+D',  data:[</v>
+      </c>
+      <c r="B27" t="str">
+        <f>B19&amp;","</f>
+        <v>55,9,</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" ref="C27:K27" si="1">C19&amp;","</f>
+        <v>55.5,</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v>48.8,</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="1"/>
+        <v>45.6,</v>
+      </c>
+      <c r="F27" t="str">
+        <f t="shared" si="1"/>
+        <v>43.8,</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="1"/>
+        <v>37.4,</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="1"/>
+        <v>32.4,</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="1"/>
+        <v>21.5,</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" si="1"/>
+        <v>17.4,</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="1"/>
+        <v>13.4,</v>
+      </c>
+      <c r="L27" t="str">
+        <f>L19&amp;"]},"</f>
+        <v>10.4]},</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f>"{name:'"&amp;A20&amp;"',  data:["</f>
+        <v>{name:'Empresas que No Invirtieron en I+D',  data:[</v>
+      </c>
+      <c r="B28" t="str">
+        <f>B20&amp;","</f>
+        <v>56,0,</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" ref="C28:K28" si="2">C20&amp;","</f>
+        <v>49.2,</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="2"/>
+        <v>42.1,</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="2"/>
+        <v>34.4,</v>
+      </c>
+      <c r="F28" t="str">
+        <f t="shared" si="2"/>
+        <v>44.0,</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="2"/>
+        <v>34.4,</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="2"/>
+        <v>38.0,</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="2"/>
+        <v>34.4,</v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" si="2"/>
+        <v>36.8,</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="2"/>
+        <v>12.8,</v>
+      </c>
+      <c r="L28" t="str">
+        <f>L20&amp;"]},"</f>
+        <v>6.4]},</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>